<commit_message>
Updating extentreport logic & Master executor
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5403696-3F77-4F11-B270-3813B434C23A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45ABE2-2B57-408E-8656-7DA4F160A002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,7 +292,7 @@
     <t>TC38_demoTestcase</t>
   </si>
   <si>
-    <t>No</t>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -1367,7 +1367,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updating testcases in Master executor
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45ABE2-2B57-408E-8656-7DA4F160A002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152CAAB-D1E0-41D1-949B-12A400F2D8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1367,7 +1367,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Updating testcases in master
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152CAAB-D1E0-41D1-949B-12A400F2D8F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02A3E2F-4295-4284-BBB2-8761CA0F7236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="83">
   <si>
     <t>Runmode</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>TC38_demoTestcase</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -780,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,7 +844,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -867,7 +864,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -887,7 +884,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
@@ -907,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
@@ -927,7 +924,7 @@
         <v>68</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -947,7 +944,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -967,7 +964,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>11</v>
@@ -987,7 +984,7 @@
         <v>29</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
@@ -1007,7 +1004,7 @@
         <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -1027,7 +1024,7 @@
         <v>41</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -1047,7 +1044,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>11</v>
@@ -1067,7 +1064,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>11</v>
@@ -1087,7 +1084,7 @@
         <v>47</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>11</v>
@@ -1107,7 +1104,7 @@
         <v>49</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>11</v>
@@ -1127,7 +1124,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>11</v>
@@ -1147,7 +1144,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>11</v>
@@ -1167,7 +1164,7 @@
         <v>53</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
@@ -1187,7 +1184,7 @@
         <v>58</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -1207,7 +1204,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>11</v>
@@ -1227,7 +1224,7 @@
         <v>66</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
@@ -1247,7 +1244,7 @@
         <v>33</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>11</v>
@@ -1267,7 +1264,7 @@
         <v>60</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>
@@ -1287,7 +1284,7 @@
         <v>66</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>11</v>
@@ -1307,7 +1304,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>11</v>
@@ -1327,7 +1324,7 @@
         <v>55</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>11</v>
@@ -1347,7 +1344,7 @@
         <v>24</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>11</v>
@@ -1387,7 +1384,7 @@
         <v>22</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>11</v>
@@ -1407,7 +1404,7 @@
         <v>62</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
@@ -1427,7 +1424,7 @@
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>11</v>
@@ -1447,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>11</v>
@@ -1467,7 +1464,7 @@
         <v>73</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>11</v>
@@ -1487,7 +1484,7 @@
         <v>78</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>11</v>
@@ -1507,7 +1504,7 @@
         <v>79</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>11</v>
@@ -1527,7 +1524,7 @@
         <v>80</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>11</v>
@@ -1547,7 +1544,7 @@
         <v>81</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>11</v>
@@ -1567,7 +1564,7 @@
         <v>82</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
First two testcases for execution..
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415226F2-A4AC-4E56-8087-467BFDDD905C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658AD688-15BD-49AF-A4BC-8A2658E6F666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,7 +739,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E32"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -805,7 +805,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Registered User testcase enable
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875BD2F-6C6C-4CC5-8BCE-7E6A47C0FEEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EC4711-75E7-4E3B-82D6-52B5319E2A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="73">
   <si>
     <t>Runmode</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>TC02_Verify_MYACC</t>
@@ -406,7 +403,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A444948E-6AA8-45F3-AB40-38513383CF85}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -881,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -948,7 +965,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -1362,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>68</v>
@@ -1388,7 +1405,7 @@
         <v>69</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
@@ -1556,42 +1573,45 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="12" priority="20"/>
+    <cfRule type="uniqueValues" dxfId="4" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="11" priority="19"/>
+    <cfRule type="uniqueValues" dxfId="14" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="10" priority="15"/>
+    <cfRule type="uniqueValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="uniqueValues" dxfId="9" priority="10"/>
+    <cfRule type="uniqueValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="8" priority="9"/>
+    <cfRule type="uniqueValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="uniqueValues" dxfId="7" priority="8"/>
+    <cfRule type="uniqueValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:F33 E2:E33">
-    <cfRule type="uniqueValues" dxfId="6" priority="7"/>
+    <cfRule type="uniqueValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="5" priority="6"/>
+    <cfRule type="uniqueValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="4" priority="5"/>
+    <cfRule type="uniqueValues" dxfId="9" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E33">
-    <cfRule type="uniqueValues" dxfId="3" priority="4"/>
+    <cfRule type="uniqueValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="uniqueValues" dxfId="2" priority="3"/>
+    <cfRule type="uniqueValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
+    <cfRule type="uniqueValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
+    <cfRule type="uniqueValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
     <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding new testcase for 20 products add to cart
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/MasterExecutor_Sanity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanCore\Input_files\Master_executors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825DDAE-7268-414A-B6F9-9C89DFE70F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429DF798-4C8A-46C5-85F0-BB70497ED460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
   <si>
     <t>Runmode</t>
   </si>
@@ -247,6 +247,13 @@
   </si>
   <si>
     <t>TC02_Verify_MYACC</t>
+  </si>
+  <si>
+    <t>1. more than 10 Items should be added to cart
+2. Appropriate inventory message must be displayed</t>
+  </si>
+  <si>
+    <t>TC39_Add_MultipleItems_to_cart</t>
   </si>
 </sst>
 </file>
@@ -387,7 +394,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A444948E-6AA8-45F3-AB40-38513383CF85}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -840,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,39 +1502,65 @@
         <v>10</v>
       </c>
     </row>
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E23">
-    <cfRule type="uniqueValues" dxfId="10" priority="20"/>
+    <cfRule type="uniqueValues" dxfId="12" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="uniqueValues" dxfId="9" priority="15"/>
+    <cfRule type="uniqueValues" dxfId="11" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="uniqueValues" dxfId="8" priority="13"/>
+    <cfRule type="uniqueValues" dxfId="10" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="uniqueValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="uniqueValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
     <cfRule type="uniqueValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E24">
     <cfRule type="uniqueValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E23">
     <cfRule type="uniqueValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E23">
     <cfRule type="uniqueValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="uniqueValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="E21:F31 E2:E32">
+    <cfRule type="uniqueValues" dxfId="3" priority="29"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="uniqueValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="E2:E32">
+    <cfRule type="uniqueValues" dxfId="2" priority="33"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F31 E2:E31">
-    <cfRule type="uniqueValues" dxfId="1" priority="27"/>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E31">
-    <cfRule type="uniqueValues" dxfId="0" priority="31"/>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="uniqueValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>